<commit_message>
Updateret tidsregistrering d. 26
</commit_message>
<xml_diff>
--- a/08-Project-Management/Tidsregistrering/Tidsregistrering (Michael).xlsx
+++ b/08-Project-Management/Tidsregistrering/Tidsregistrering (Michael).xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Michael\git\PTECalculator2015\08-Project-Management\Tidsregistrering\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Michael\Documents\GitHub\PTECalculator2015\08-Project-Management\Tidsregistrering\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="10416" windowHeight="5940"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="10410" windowHeight="5940"/>
   </bookViews>
   <sheets>
     <sheet name="Tidsregistrering" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="14">
   <si>
     <t>Navn</t>
   </si>
@@ -56,13 +56,16 @@
     <t>System Analyst</t>
   </si>
   <si>
-    <t>Samtale med Team 7 (kunden)</t>
-  </si>
-  <si>
     <t>Business-process analyst</t>
   </si>
   <si>
     <t>Lavet udkast til domænemodel for UC1/UC2 + dataordborg for UC1/UC2. Har gennemgået rettelser med anden gruppe af samme opgaver.</t>
+  </si>
+  <si>
+    <t>Samtale med Team 5 (kunden) UC5</t>
+  </si>
+  <si>
+    <t>Samtale med Team 7 (kunden) UC1+UC2</t>
   </si>
 </sst>
 </file>
@@ -401,21 +404,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.6640625" style="4" customWidth="1"/>
-    <col min="2" max="2" width="6.6640625" customWidth="1"/>
-    <col min="3" max="3" width="25.6640625" customWidth="1"/>
-    <col min="4" max="4" width="50.6640625" customWidth="1"/>
+    <col min="1" max="1" width="10.7109375" style="4" customWidth="1"/>
+    <col min="2" max="2" width="6.7109375" customWidth="1"/>
+    <col min="3" max="3" width="25.7109375" customWidth="1"/>
+    <col min="4" max="4" width="50.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -423,7 +426,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>1</v>
       </c>
@@ -437,7 +440,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="4">
         <v>42058</v>
       </c>
@@ -451,7 +454,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="4">
         <v>42059</v>
       </c>
@@ -465,7 +468,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="4">
         <v>42059</v>
       </c>
@@ -473,13 +476,13 @@
         <v>2</v>
       </c>
       <c r="C5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D5" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="4">
         <v>42059</v>
       </c>
@@ -490,7 +493,35 @@
         <v>9</v>
       </c>
       <c r="D6" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="4">
+        <v>42061</v>
+      </c>
+      <c r="B7">
+        <v>0.5</v>
+      </c>
+      <c r="C7" t="s">
+        <v>10</v>
+      </c>
+      <c r="D7" t="s">
         <v>12</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="4">
+        <v>42061</v>
+      </c>
+      <c r="B8">
+        <v>1.2</v>
+      </c>
+      <c r="C8" t="s">
+        <v>9</v>
+      </c>
+      <c r="D8" t="s">
+        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>